<commit_message>
Completed Task 1-4 working on 5-6
Working on the final 2 tasks, updated and completed tasks 1-4
</commit_message>
<xml_diff>
--- a/IDEAS AND STATUS.xlsx
+++ b/IDEAS AND STATUS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University Work (LAPTOP)\Year 2\Sem 1\SWE30011 - IoT Programming\Assignment3\Github Repo\Ultra Sonic Sensor\Ultra Sonic Sensor\Ultra_Sonic_Sensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University Work (LAPTOP)\Year 2\Sem 1\SWE30011 - IoT Programming\Assignment3\Github Repo\Ultra Sonic Sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93E282F-311F-4A65-A3D0-EF3089F6A9B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6337C58E-DA1E-487C-8BCB-2E38D61E5CB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4E371B63-0569-4965-9C47-69E6BE8DFB49}"/>
+    <workbookView xWindow="16905" yWindow="6930" windowWidth="21600" windowHeight="11505" xr2:uid="{4E371B63-0569-4965-9C47-69E6BE8DFB49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Smart Parking System (Ultra Sonic Sensor Module + possibly LED'S (as bug testing))</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Email Guide Links for 5</t>
+  </si>
+  <si>
+    <t>This smart paking system is designed for a pre setup group of people such a hotell where you have users details</t>
+  </si>
+  <si>
+    <t>Admin Login Area To Set Price?</t>
   </si>
 </sst>
 </file>
@@ -438,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478E5D64-AE23-47D1-9CAD-D389CDE23F86}">
-  <dimension ref="B4:F19"/>
+  <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +456,11 @@
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>0</v>
@@ -470,6 +481,9 @@
       <c r="B6">
         <v>1</v>
       </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -509,6 +523,9 @@
       <c r="B9">
         <v>4</v>
       </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
       <c r="E9">
         <v>4</v>
       </c>
@@ -536,6 +553,11 @@
       </c>
       <c r="F11" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished Task 5 (Email Send)
Current bug - reloading page auto re sends email
Possible fix = database variable 1 = DONT SEND 0 = SEND

To Implement ADMIN LOGIN AREA
</commit_message>
<xml_diff>
--- a/IDEAS AND STATUS.xlsx
+++ b/IDEAS AND STATUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University Work (LAPTOP)\Year 2\Sem 1\SWE30011 - IoT Programming\Assignment3\Github Repo\Ultra Sonic Sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6337C58E-DA1E-487C-8BCB-2E38D61E5CB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F625D9-F5F1-4815-93BE-DE6902E25B51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16905" yWindow="6930" windowWidth="21600" windowHeight="11505" xr2:uid="{4E371B63-0569-4965-9C47-69E6BE8DFB49}"/>
+    <workbookView xWindow="38100" yWindow="1545" windowWidth="21600" windowHeight="11505" xr2:uid="{4E371B63-0569-4965-9C47-69E6BE8DFB49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Smart Parking System (Ultra Sonic Sensor Module + possibly LED'S (as bug testing))</t>
   </si>
@@ -51,15 +51,6 @@
     <t xml:space="preserve">•For cloud: regression machine learning model to predict the availability of car park space etc. </t>
   </si>
   <si>
-    <t xml:space="preserve">I May add or remove things from this assignment depending on both time/difficulty. </t>
-  </si>
-  <si>
-    <t>How To Setup Email Function PHP:  https://www.w3schools.com/php/func_mail_mail.asp</t>
-  </si>
-  <si>
-    <t>How To Setup gmail SMTP server form PHP: https://stackoverflow.com/questions/712392/send-email-using-the-gmail-smtp-server-from-a-php-page</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -75,13 +66,7 @@
     <t>IDEA #</t>
   </si>
   <si>
-    <t>Email Guide Links for 5</t>
-  </si>
-  <si>
     <t>This smart paking system is designed for a pre setup group of people such a hotell where you have users details</t>
-  </si>
-  <si>
-    <t>Admin Login Area To Set Price?</t>
   </si>
 </sst>
 </file>
@@ -444,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478E5D64-AE23-47D1-9CAD-D389CDE23F86}">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +443,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -468,13 +453,13 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -482,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -496,13 +481,13 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -510,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -524,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -537,6 +522,9 @@
       <c r="B10">
         <v>5</v>
       </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
       <c r="E10">
         <v>5</v>
       </c>
@@ -555,33 +543,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>